<commit_message>
Pushing new version to remote
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sezer\Documents\UiPath\CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4013B5-EA3B-4E63-87B5-9C5C1C29BA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FAC1E8-1287-4D4E-B9D4-8678509E2484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="705" windowWidth="17025" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -588,7 +588,7 @@
   <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>